<commit_message>
create mock setup for testing external dependencies
</commit_message>
<xml_diff>
--- a/Doc/JDT-Thibaud.xlsx
+++ b/Doc/JDT-Thibaud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaudracine/Documents/GitHub/324_portfolio_app1_Racine-Thibaud/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26EC5FFC-D68F-DD42-A2F1-499DF7DC2159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E5A24-5991-7C4D-895B-E57878C7DB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17240" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Auteur:</t>
   </si>
@@ -158,6 +158,60 @@
   </si>
   <si>
     <t>Lecture du cahier des charges et prise de notes</t>
+  </si>
+  <si>
+    <t>Malade</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>Recherche d'une deuxième app pour le portfolio.</t>
+  </si>
+  <si>
+    <t>Création du repo pour la deuxième app Flask Login System</t>
+  </si>
+  <si>
+    <t>Mise en page de la documentation sur un fichier Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration de l'environnement de développement </t>
+  </si>
+  <si>
+    <t>Documentation de la mise en place et configuration de l'environnement de développement</t>
+  </si>
+  <si>
+    <t>Configuration ID Gecko, Création du fichier TODO sur OneDrive et install des dépendances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déployement de l'addon Firefox </t>
+  </si>
+  <si>
+    <t>Génération des clés API et ajout du code source</t>
+  </si>
+  <si>
+    <t>Documentation sur le déployement de l'addon Firefox</t>
+  </si>
+  <si>
+    <t>Mise en place de l'environnement de tests pour l'addon FireFox</t>
+  </si>
+  <si>
+    <t>Installation de Vitest et node pour les Tests unitaires</t>
+  </si>
+  <si>
+    <t>Documentation sur la mise en place de l'environnement de tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place du GitHub Action pour automatiser les tests </t>
+  </si>
+  <si>
+    <t>J'ai ajouté un bête test pour voir si cela fonctionnait</t>
+  </si>
+  <si>
+    <t>Documentation sur la mise en place de GitHub Action</t>
+  </si>
+  <si>
+    <t>Sauvegarde du cache et artifact automatique avec GitHub Action</t>
   </si>
 </sst>
 </file>
@@ -288,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +415,18 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -398,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -612,11 +678,122 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1124,13 +1301,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1976,13 +2153,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.36046511627906974</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.63953488372093026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3960,23 +4137,19 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="22">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4171,8 +4344,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4183,7 +4356,7 @@
     <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="83.5" customWidth="1"/>
-    <col min="7" max="7" width="72.1640625" customWidth="1"/>
+    <col min="7" max="7" width="86.83203125" customWidth="1"/>
     <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -4227,7 +4400,7 @@
       <c r="B3" s="87"/>
       <c r="C3" s="76" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 0 minutes</v>
+        <v>8 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4246,11 +4419,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>180</v>
+        <v>485</v>
       </c>
       <c r="E4" s="27">
         <f>SUM(C4:D4)</f>
-        <v>180</v>
+        <v>485</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4516,228 +4689,345 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="71" t="str">
+    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="71">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="B16" s="34">
+        <v>45635</v>
+      </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="36">
+        <v>20</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="G16" s="43"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="72" t="str">
+    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="72">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="38"/>
+        <v>50</v>
+      </c>
+      <c r="B17" s="38">
+        <v>45635</v>
+      </c>
       <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="44"/>
+      <c r="D17" s="40">
+        <v>30</v>
+      </c>
+      <c r="E17" s="96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>46</v>
+      </c>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="71" t="str">
+    <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="71">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="B18" s="34">
+        <v>45635</v>
+      </c>
       <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="26"/>
+      <c r="D18" s="36">
+        <v>15</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="G18" s="43"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="72" t="str">
+    <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="72">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="38"/>
+        <v>50</v>
+      </c>
+      <c r="B19" s="38">
+        <v>45635</v>
+      </c>
       <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="44"/>
+      <c r="D19" s="40">
+        <v>20</v>
+      </c>
+      <c r="E19" s="96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="71" t="str">
+    <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="71">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="B20" s="34">
+        <v>45635</v>
+      </c>
       <c r="C20" s="35"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="26"/>
+      <c r="D20" s="36">
+        <v>15</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="G20" s="43"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="72" t="str">
+      <c r="A21" s="78" t="str">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
         <v/>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="44"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="71" t="str">
+      <c r="B21" s="79"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
+    </row>
+    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="71">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="B22" s="34">
+        <v>45638</v>
+      </c>
       <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="26"/>
+      <c r="D22" s="36">
+        <v>55</v>
+      </c>
+      <c r="E22" s="94" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="G22" s="43"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="72" t="str">
+      <c r="A23" s="78" t="str">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
         <v/>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="44"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="71" t="str">
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="84"/>
+    </row>
+    <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="71">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="B24" s="34">
+        <v>45642</v>
+      </c>
       <c r="C24" s="35"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="26"/>
+      <c r="D24" s="36">
+        <v>20</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="G24" s="43"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="72" t="str">
+    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="72">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B25" s="38">
+        <v>45642</v>
+      </c>
       <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="26"/>
+      <c r="D25" s="40">
+        <v>10</v>
+      </c>
+      <c r="E25" s="96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="G25" s="44"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="71" t="str">
+    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="71">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="B26" s="34">
+        <v>45642</v>
+      </c>
       <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="43"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="72" t="str">
+      <c r="D26" s="36">
+        <v>20</v>
+      </c>
+      <c r="E26" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="72">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B27" s="38">
+        <v>45642</v>
+      </c>
       <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="44"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="71" t="str">
+      <c r="D27" s="40">
+        <v>10</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="71">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="B28" s="34">
+        <v>45642</v>
+      </c>
       <c r="C28" s="35"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="25"/>
+      <c r="D28" s="36">
+        <v>45</v>
+      </c>
+      <c r="E28" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="98" t="s">
+        <v>53</v>
+      </c>
       <c r="G28" s="43"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="72" t="str">
+      <c r="A29" s="72">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B29" s="38">
+        <v>45642</v>
+      </c>
       <c r="C29" s="39"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="40">
+        <v>15</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G29" s="44"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="71" t="str">
+      <c r="A30" s="8" t="str">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
         <v/>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="43"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="92"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="72" t="str">
+      <c r="A31" s="72">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B31" s="38">
+        <v>45645</v>
+      </c>
       <c r="C31" s="39"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="40">
+        <v>30</v>
+      </c>
+      <c r="E31" s="96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="G31" s="44"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="71" t="str">
+      <c r="A32" s="71">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="B32" s="34">
+        <v>45645</v>
+      </c>
       <c r="C32" s="35"/>
       <c r="D32" s="36"/>
       <c r="E32" s="37"/>
       <c r="F32" s="26"/>
       <c r="G32" s="43"/>
+      <c r="H32" s="36"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="72" t="str">
+      <c r="A33" s="72">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B33" s="38">
+        <v>45645</v>
+      </c>
       <c r="C33" s="39"/>
       <c r="D33" s="40"/>
       <c r="E33" s="41"/>
@@ -4745,40 +5035,44 @@
       <c r="G33" s="44"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="71" t="str">
+      <c r="A34" s="71">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="B34" s="34">
+        <v>45645</v>
+      </c>
       <c r="C34" s="35"/>
-      <c r="D34" s="36"/>
+      <c r="D34" s="93"/>
       <c r="E34" s="37"/>
       <c r="F34" s="25"/>
       <c r="G34" s="43"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="72" t="str">
+      <c r="A35" s="72">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B35" s="38">
+        <v>45645</v>
+      </c>
       <c r="C35" s="39"/>
-      <c r="D35" s="40"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="41"/>
       <c r="F35" s="26"/>
       <c r="G35" s="44"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="71" t="str">
+      <c r="A36" s="8" t="str">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
         <v/>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="43"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="92"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="72" t="str">
@@ -10740,41 +11034,67 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="E7:E21 E23:E532">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="7" priority="18">
+      <formula>$D35="Autre"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="19" stopIfTrue="1">
+      <formula>$D35="Design"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="20" stopIfTrue="1">
+      <formula>$D35="Présentation"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="21" stopIfTrue="1">
+      <formula>$D35="Meeting"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="22" stopIfTrue="1">
+      <formula>$D35="Documentation"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="23" stopIfTrue="1">
+      <formula>$D35="Test"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="24" stopIfTrue="1">
+      <formula>$D35="Analyse"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="25" stopIfTrue="1">
+      <formula>$D35="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E21 E23:E532 D35" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
+      <formula1>$M$7:$M$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D33 D35:D532 H32" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
       <formula1>$O$7:$O$19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
-      <formula1>$M$7:$M$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10791,7 +11111,7 @@
   <dimension ref="A2:N12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D8" sqref="A8:XFD8"/>
+      <selection activeCell="D7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -10909,11 +11229,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="E7" s="28" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10921,11 +11241,11 @@
       </c>
       <c r="F7" s="53" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>2 h 35 min</v>
       </c>
       <c r="G7" s="54">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0</v>
+        <v>0.36046511627906974</v>
       </c>
       <c r="L7" s="62" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10983,11 +11303,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>180</v>
+        <v>275</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>275</v>
       </c>
       <c r="E9" s="21" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10995,11 +11315,11 @@
       </c>
       <c r="F9" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 00 min</v>
+        <v>4 h 35 min</v>
       </c>
       <c r="G9" s="54">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.63953488372093026</v>
       </c>
       <c r="L9" s="64" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11020,22 +11340,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>180</v>
+        <v>430</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>180</v>
+        <v>430</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 00 min</v>
+        <v>7 h 10 min</v>
       </c>
       <c r="G10" s="55">
         <f>C10/C11</f>
-        <v>3.4090909090909088E-2</v>
+        <v>8.1439393939393936E-2</v>
       </c>
       <c r="L10" s="65" t="s">
         <v>18</v>
@@ -11056,7 +11376,6 @@
       <c r="F12" s="49"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uUegAJ0zdAusDcOf3en73L5ZNP0cz+qyzL+KwkOPao3aJqynoKuocLlsQrShjMwrq5gdKGShXjoYCXvDreYtSg==" saltValue="o84qDdvSZ3Es6qbaOlmJjQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -11079,6 +11398,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="438c9102f2c873572ee53782e3c89f23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7be26b22cb6e6d4b7374fec5a60b7d" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11273,17 +11603,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11294,6 +11613,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0FE8E31-C0A2-4F58-8D4B-0B811B1C703F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11312,23 +11648,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>

</xml_diff>